<commit_message>
FAAS-459 iOS phone Device testing
</commit_message>
<xml_diff>
--- a/src/test/resources/FHEO-Shakeoutdata.xlsx
+++ b/src/test/resources/FHEO-Shakeoutdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\krish\IdeaProjects\formservice-testing\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63BB2ED2-53A9-49C9-B89C-5368F1E9C19E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6596670-07A0-4B57-BF52-ED6948ABDD58}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" tabRatio="474" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="62">
   <si>
     <t>race</t>
   </si>
@@ -217,6 +217,9 @@
   </si>
   <si>
     <t>05-12-2021</t>
+  </si>
+  <si>
+    <t>discDateWithTimestamp</t>
   </si>
 </sst>
 </file>
@@ -1156,13 +1159,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AK2"/>
+  <dimension ref="A1:AL2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="N2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="AF2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="T2" sqref="T2"/>
+      <selection pane="bottomRight" activeCell="AK6" sqref="AK6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1207,7 +1210,7 @@
     <col min="38" max="16384" width="8.83984375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:38" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1319,8 +1322,11 @@
       <c r="AK1" s="14" t="s">
         <v>51</v>
       </c>
+      <c r="AL1" s="2" t="s">
+        <v>61</v>
+      </c>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:38" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="19" t="s">
         <v>6</v>
       </c>

</xml_diff>